<commit_message>
Create pointsale and tickets
</commit_message>
<xml_diff>
--- a/public/plantillas/PlantillaDeProductos.xlsx
+++ b/public/plantillas/PlantillaDeProductos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jose_\Desktop\vue y laravel\presupuesto\public\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{860E7E0E-391B-40AE-9531-81EAABB9E5D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35182D93-477A-49BC-968B-71CDC016CDB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D7F0C672-DFC9-458F-B1D8-AC26D37570F7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Nombre del producto</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>Peso</t>
+  </si>
+  <si>
+    <t>Tiene IVA</t>
+  </si>
+  <si>
+    <t>¿Es producto?</t>
   </si>
 </sst>
 </file>
@@ -421,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34CC209C-F11B-43B5-91A5-83469129EF88}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -435,7 +441,7 @@
     <col min="9" max="10" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -474,6 +480,12 @@
       </c>
       <c r="M1" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>